<commit_message>
Credits Screen code + new Main Menu image
</commit_message>
<xml_diff>
--- a/JetpackArcher/Documentation/Environment Collision Rects.xlsx
+++ b/JetpackArcher/Documentation/Environment Collision Rects.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>Rect</t>
   </si>
@@ -60,6 +60,15 @@
   </si>
   <si>
     <t>Menu Box</t>
+  </si>
+  <si>
+    <t>Quit Main Menu</t>
+  </si>
+  <si>
+    <t>Back Credit Screen</t>
+  </si>
+  <si>
+    <t>Credit Screen</t>
   </si>
 </sst>
 </file>
@@ -409,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1049,6 +1058,46 @@
         <v>11</v>
       </c>
     </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" s="5">
+        <v>430</v>
+      </c>
+      <c r="C35" s="5">
+        <v>668</v>
+      </c>
+      <c r="D35" s="5">
+        <v>158</v>
+      </c>
+      <c r="E35" s="5">
+        <v>70</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B36" s="5">
+        <v>428</v>
+      </c>
+      <c r="C36" s="5">
+        <v>668</v>
+      </c>
+      <c r="D36" s="5">
+        <v>198</v>
+      </c>
+      <c r="E36" s="5">
+        <v>68</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Game Over Screen + Small bug Fix
Fixed a state setting error in JetpackAracher.cpp
</commit_message>
<xml_diff>
--- a/JetpackArcher/Documentation/Environment Collision Rects.xlsx
+++ b/JetpackArcher/Documentation/Environment Collision Rects.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>Rect</t>
   </si>
@@ -69,6 +69,15 @@
   </si>
   <si>
     <t>Credit Screen</t>
+  </si>
+  <si>
+    <t>Game Over Screen</t>
+  </si>
+  <si>
+    <t>Try Again button</t>
+  </si>
+  <si>
+    <t>Quit Game Over</t>
   </si>
 </sst>
 </file>
@@ -92,12 +101,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -127,7 +142,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -138,6 +153,10 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1019,37 +1038,25 @@
       <c r="F32" s="2"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B33" s="5">
-        <v>350</v>
-      </c>
-      <c r="C33" s="5">
-        <v>416</v>
-      </c>
-      <c r="D33" s="5">
-        <v>320</v>
-      </c>
-      <c r="E33" s="5">
-        <v>96</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="A33" s="6"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B34" s="2">
+        <v>9</v>
+      </c>
+      <c r="B34" s="5">
+        <v>350</v>
+      </c>
+      <c r="C34" s="5">
+        <v>416</v>
+      </c>
+      <c r="D34" s="5">
         <v>320</v>
-      </c>
-      <c r="C34" s="2">
-        <v>512</v>
-      </c>
-      <c r="D34" s="5">
-        <v>384</v>
       </c>
       <c r="E34" s="5">
         <v>96</v>
@@ -1060,19 +1067,19 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B35" s="5">
-        <v>430</v>
-      </c>
-      <c r="C35" s="5">
-        <v>668</v>
+        <v>10</v>
+      </c>
+      <c r="B35" s="2">
+        <v>320</v>
+      </c>
+      <c r="C35" s="2">
+        <v>512</v>
       </c>
       <c r="D35" s="5">
-        <v>158</v>
+        <v>384</v>
       </c>
       <c r="E35" s="5">
-        <v>70</v>
+        <v>96</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>11</v>
@@ -1080,22 +1087,82 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B36" s="5">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="C36" s="5">
         <v>668</v>
       </c>
       <c r="D36" s="5">
+        <v>158</v>
+      </c>
+      <c r="E36" s="5">
+        <v>70</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B37" s="5">
+        <v>428</v>
+      </c>
+      <c r="C37" s="5">
+        <v>668</v>
+      </c>
+      <c r="D37" s="5">
         <v>198</v>
       </c>
-      <c r="E36" s="5">
+      <c r="E37" s="5">
         <v>68</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="F37" s="2" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B38" s="5">
+        <v>384</v>
+      </c>
+      <c r="C38" s="5">
+        <v>300</v>
+      </c>
+      <c r="D38" s="5">
+        <v>288</v>
+      </c>
+      <c r="E38" s="5">
+        <v>58</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B39" s="5">
+        <v>460</v>
+      </c>
+      <c r="C39" s="5">
+        <v>376</v>
+      </c>
+      <c r="D39" s="5">
+        <v>144</v>
+      </c>
+      <c r="E39" s="5">
+        <v>58</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Game Won screen + arrow drawing fix
</commit_message>
<xml_diff>
--- a/JetpackArcher/Documentation/Environment Collision Rects.xlsx
+++ b/JetpackArcher/Documentation/Environment Collision Rects.xlsx
@@ -449,7 +449,7 @@
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1179,16 +1179,16 @@
         <v>20</v>
       </c>
       <c r="B40" s="5">
-        <v>336</v>
+        <v>314</v>
       </c>
       <c r="C40" s="5">
-        <v>300</v>
+        <v>394</v>
       </c>
       <c r="D40" s="5">
-        <v>288</v>
+        <v>390</v>
       </c>
       <c r="E40" s="5">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="F40" s="5" t="s">
         <v>19</v>
@@ -1199,16 +1199,16 @@
         <v>18</v>
       </c>
       <c r="B41" s="5">
-        <v>460</v>
+        <v>426</v>
       </c>
       <c r="C41" s="5">
-        <v>300</v>
+        <v>458</v>
       </c>
       <c r="D41" s="5">
-        <v>412</v>
+        <v>166</v>
       </c>
       <c r="E41" s="5">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F41" s="5" t="s">
         <v>19</v>

</xml_diff>